<commit_message>
adding file of nonstandard vars for data dict
</commit_message>
<xml_diff>
--- a/src/sdmc_adhoc_processing/data_dictionary_TEMPLATE.xlsx
+++ b/src/sdmc_adhoc_processing/data_dictionary_TEMPLATE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\vtn\lab\SDMC_labscience\operations\documents\templates\assay\template_testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhaddock\DOCUME~1\MobaXterm\slash\RemoteFiles\133792_3_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDAABDE-3675-4B9C-92F1-033C64DD8B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0794004-CC85-4D68-A6C6-F6516B235569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15540" yWindow="-16200" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15540" yWindow="-16200" windowWidth="22785" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="draft_data_dictionary" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
   <si>
     <t>variable_name</t>
   </si>
@@ -225,6 +225,15 @@
   </si>
   <si>
     <t>lab_software_version</t>
+  </si>
+  <si>
+    <t>assay_details</t>
+  </si>
+  <si>
+    <t>result_units</t>
+  </si>
+  <si>
+    <t>Units corresponding to result</t>
   </si>
 </sst>
 </file>
@@ -1095,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1336,75 +1345,96 @@
     </row>
     <row r="17" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>28</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="B17" s="8"/>
       <c r="C17" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="7"/>
+      <c r="E17" s="10"/>
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="E18" s="7"/>
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B19" s="6"/>
       <c r="E19" s="7"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="20" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="C22" t="s">
         <v>19</v>
       </c>
-      <c r="D22" t="s">
+      <c r="F22" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>